<commit_message>
Update of experiment results
</commit_message>
<xml_diff>
--- a/benchmark/experiments/adding_headers_to_samples (rf@charfreq model, 10 runs per p_header value) [30-01-2017].xlsx
+++ b/benchmark/experiments/adding_headers_to_samples (rf@charfreq model, 10 runs per p_header value) [30-01-2017].xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="42780" yWindow="1180" windowWidth="28840" windowHeight="18600"/>
+    <workbookView xWindow="4380" yWindow="8460" windowWidth="28840" windowHeight="14420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4740,7 +4740,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>